<commit_message>
thay đôi chiến lược chạy multi process. Sửa lại template báo cáo tổng hợp cơ sở
</commit_message>
<xml_diff>
--- a/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-29 Lâm Hoàng Phú 8-2024.xlsx
+++ b/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-29 Lâm Hoàng Phú 8-2024.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -534,20 +534,106 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>620</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>08-03-2024</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Trần Thị Thanh Nhàn</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Cá nhân</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Nâng mũi</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Lâm Hoàng Phú</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>HD-LUXURY</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>621</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>08-03-2024</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Trần Thị Ngọc Dung</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Cá nhân</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Nâng mũi</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Lâm Hoàng Phú</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>Tổng</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
-      <c r="I3" t="n">
-        <v>50000</v>
+      <c r="B5" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="n">
+        <v>250000</v>
       </c>
     </row>
   </sheetData>
@@ -596,7 +682,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>285714.2857142857</v>
+        <v>232142.8571428571</v>
       </c>
     </row>
     <row r="4">
@@ -646,7 +732,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>50000</v>
+        <v>250000</v>
       </c>
     </row>
     <row r="9">
@@ -876,7 +962,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>335714.2857142857</v>
+        <v>482142.8571428572</v>
       </c>
     </row>
     <row r="32">
@@ -906,7 +992,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>335714.2857142857</v>
+        <v>482142.8571428572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tổng hợp thưởng phạt trong report cá nhân
</commit_message>
<xml_diff>
--- a/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-29 Lâm Hoàng Phú 8-2024.xlsx
+++ b/Báo cáo/1_CẦN THƠ/Báo cáo cá nhân/NV-29 Lâm Hoàng Phú 8-2024.xlsx
@@ -9,7 +9,8 @@
   <sheets>
     <sheet name="Đơn sale chính" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Đơn phụ phẫu 1" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Lương" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Thưởng" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Lương" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -647,7 +648,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -658,6 +659,143 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Ngày phát sinh</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notion id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Tiền tố</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Mã thưởng phạt</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>id nhân sự</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Cơ sở</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Loại</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Lượng thưởng phạt</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Lí do</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Họ và tên</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>08-05-2024</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>f1df828e-4b4e-4cec-93fb-1de41e0d82f5</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>TP</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>9</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>e49d0ce3-124d-4e4b-b377-be2139cde3f5</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>CẦN THƠ</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Thưởng</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>4000000</v>
+      </c>
+      <c r="I2" t="n">
+        <v/>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>Lâm Hoàng Phú</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Tổng</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="n">
+        <v>4000000</v>
+      </c>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
           <t>Danh mục lương</t>
         </is>
       </c>
@@ -758,17 +896,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Tổng công tại LONG XUYÊN</t>
+          <t>Thưởng tại CẦN THƠ</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Lương công tác tại LONG XUYÊN</t>
+          <t>Tổng công tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -778,27 +916,27 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Lương cơ bản tại LONG XUYÊN</t>
+          <t>Lương công tác tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Chiết khấu sale chính tại LONG XUYÊN</t>
+          <t>Lương cơ bản tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Chiết khấu sale phụ tại LONG XUYÊN</t>
+          <t>Chiết khấu sale chính tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -808,7 +946,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Đơn 1 bác sĩ tại LONG XUYÊN</t>
+          <t>Chiết khấu sale phụ tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -818,7 +956,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Đơn 2 bác sĩ tại LONG XUYÊN</t>
+          <t>Đơn 1 bác sĩ tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -828,7 +966,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Công phụ phẫu 1 tại LONG XUYÊN</t>
+          <t>Đơn 2 bác sĩ tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -838,7 +976,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Công phụ phẫu 2 tại LONG XUYÊN</t>
+          <t>Công phụ phẫu 1 tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -848,7 +986,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Ứng lương tại LONG XUYÊN</t>
+          <t>Công phụ phẫu 2 tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -858,7 +996,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Tổng công tại SÓC TRĂNG</t>
+          <t>Ứng lương tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -868,7 +1006,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Lương công tác tại SÓC TRĂNG</t>
+          <t>Tổng công tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -878,27 +1016,27 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Lương cơ bản tại SÓC TRĂNG</t>
+          <t>Lương công tác tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v/>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Chiết khấu sale chính tại SÓC TRĂNG</t>
+          <t>Lương cơ bản tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v/>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Chiết khấu sale phụ tại SÓC TRĂNG</t>
+          <t>Chiết khấu sale chính tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -908,7 +1046,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Đơn 1 bác sĩ tại SÓC TRĂNG</t>
+          <t>Chiết khấu sale phụ tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -918,7 +1056,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Đơn 2 bác sĩ tại SÓC TRĂNG</t>
+          <t>Đơn 1 bác sĩ tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -928,7 +1066,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Công phụ phẫu 1 tại SÓC TRĂNG</t>
+          <t>Đơn 2 bác sĩ tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -938,7 +1076,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Công phụ phẫu 2 tại SÓC TRĂNG</t>
+          <t>Công phụ phẫu 1 tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -948,7 +1086,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Ứng lương tại SÓC TRĂNG</t>
+          <t>Công phụ phẫu 2 tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -958,27 +1096,27 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Tổng lương tại CẦN THƠ</t>
+          <t>Ứng lương tại SÓC TRĂNG</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>482142.8571428572</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Tổng lương tại LONG XUYÊN</t>
+          <t>Tổng lương tại CẦN THƠ</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>4482142.857142857</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Tổng lương tại SÓC TRĂNG</t>
+          <t>Tổng lương tại LONG XUYÊN</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -988,11 +1126,21 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>Tổng lương tại SÓC TRĂNG</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>Tổng lương tại HỆ THỐNG</t>
         </is>
       </c>
-      <c r="B34" t="n">
-        <v>482142.8571428572</v>
+      <c r="B35" t="n">
+        <v>4482142.857142857</v>
       </c>
     </row>
   </sheetData>

</xml_diff>